<commit_message>
Deploy versión estable desde local
</commit_message>
<xml_diff>
--- a/JUGADORES T1.xlsx
+++ b/JUGADORES T1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\pingpong_full\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bots\pp_consulta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74EC4803-78B8-41E3-A2D5-E0F154699B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F474921E-9175-4166-A98F-B2D8746F860D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A98060DC-1932-43E6-9169-0378406E7D7E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{A98060DC-1932-43E6-9169-0378406E7D7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>DIV 1</t>
-  </si>
-  <si>
-    <t>DIV 2</t>
-  </si>
-  <si>
-    <t>DIV 3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Rubén Serna</t>
   </si>
@@ -451,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3AEB69-7505-4905-87B6-66EA901D9D74}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,92 +460,81 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>